<commit_message>
BOM checked against recieved parts and ommisions noted
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="165">
   <si>
     <t xml:space="preserve">QTY </t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">47u</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">1276-1000-6-ND</t>
   </si>
   <si>
@@ -61,6 +64,9 @@
     <t xml:space="preserve">100n</t>
   </si>
   <si>
+    <t xml:space="preserve">didn’t get counted, probably 40</t>
+  </si>
+  <si>
     <t xml:space="preserve">1276-1119-1-ND</t>
   </si>
   <si>
@@ -88,6 +94,12 @@
     <t xml:space="preserve">1u</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">SML-H12P8TT86CCT-ND</t>
   </si>
   <si>
@@ -163,10 +175,7 @@
     <t xml:space="preserve">hdmi</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Got miniHDMI, might have meant to order full size?</t>
+    <t xml:space="preserve">Got miniHDMI, meant to order that</t>
   </si>
   <si>
     <t xml:space="preserve">952-2262-ND</t>
@@ -286,6 +295,9 @@
     <t xml:space="preserve">0 ohm</t>
   </si>
   <si>
+    <t xml:space="preserve">As 12+18 in separate bags</t>
+  </si>
+  <si>
     <t xml:space="preserve">RG16P100BCT-ND</t>
   </si>
   <si>
@@ -334,6 +346,9 @@
     <t xml:space="preserve">1.75k</t>
   </si>
   <si>
+    <t xml:space="preserve">Got 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">RMCF0603FT27K0CT-ND</t>
   </si>
   <si>
@@ -352,6 +367,9 @@
     <t xml:space="preserve">56.2k</t>
   </si>
   <si>
+    <t xml:space="preserve">none arrived</t>
+  </si>
+  <si>
     <t xml:space="preserve">311-47.0KHRCT-ND</t>
   </si>
   <si>
@@ -458,6 +476,9 @@
   </si>
   <si>
     <t xml:space="preserve">FSUSB42UMX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Help us!!! These are going to be a nightmare to solder</t>
   </si>
   <si>
     <t xml:space="preserve">A118230CT-ND</t>
@@ -593,8 +614,8 @@
   </sheetPr>
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J46" activeCellId="0" sqref="J46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -602,7 +623,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.53"/>
@@ -654,6 +676,9 @@
         <f aca="false">H2*G2</f>
         <v>6.4</v>
       </c>
+      <c r="J2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -663,13 +688,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>0.025</v>
@@ -680,6 +705,12 @@
       <c r="I3" s="0" t="n">
         <f aca="false">H3*G3</f>
         <v>1</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,13 +721,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>0.099</v>
@@ -708,6 +739,9 @@
         <f aca="false">H4*G4</f>
         <v>0.99</v>
       </c>
+      <c r="J4" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -717,13 +751,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>0.62</v>
@@ -735,6 +769,9 @@
         <f aca="false">H5*G5</f>
         <v>2.48</v>
       </c>
+      <c r="J5" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -744,13 +781,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>0.022</v>
@@ -762,6 +799,12 @@
         <f aca="false">H6*G6</f>
         <v>0.22</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -771,13 +814,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>0.2068</v>
@@ -789,6 +832,9 @@
         <f aca="false">H7*G7</f>
         <v>5.7904</v>
       </c>
+      <c r="J7" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -798,13 +844,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>0.68</v>
@@ -816,22 +862,25 @@
         <f aca="false">H8*G8</f>
         <v>3.4</v>
       </c>
+      <c r="J8" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>0.329</v>
@@ -843,22 +892,25 @@
         <f aca="false">H9*G9</f>
         <v>3.29</v>
       </c>
+      <c r="J9" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="false">H10*G10</f>
@@ -873,13 +925,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>0.58</v>
@@ -891,6 +943,9 @@
         <f aca="false">H11*G11</f>
         <v>2.9</v>
       </c>
+      <c r="J11" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -900,13 +955,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>0.37</v>
@@ -918,6 +973,9 @@
         <f aca="false">H12*G12</f>
         <v>1.85</v>
       </c>
+      <c r="J12" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -927,13 +985,13 @@
         <v>6</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>0.76</v>
@@ -945,6 +1003,12 @@
         <f aca="false">H13*G13</f>
         <v>2.28</v>
       </c>
+      <c r="J13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -954,13 +1018,13 @@
         <v>6</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>2.3</v>
@@ -973,10 +1037,10 @@
         <v>13.8</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -987,13 +1051,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>0.08</v>
@@ -1005,6 +1069,9 @@
         <f aca="false">H15*G15</f>
         <v>0.32</v>
       </c>
+      <c r="J15" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1014,13 +1081,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>0.1</v>
@@ -1032,6 +1099,9 @@
         <f aca="false">H16*G16</f>
         <v>0.2</v>
       </c>
+      <c r="J16" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -1041,13 +1111,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>0.14</v>
@@ -1059,6 +1129,9 @@
         <f aca="false">H17*G17</f>
         <v>0.28</v>
       </c>
+      <c r="J17" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -1068,13 +1141,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>0.2</v>
@@ -1086,6 +1159,9 @@
         <f aca="false">H18*G18</f>
         <v>0.4</v>
       </c>
+      <c r="J18" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -1095,13 +1171,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>0.26</v>
@@ -1113,6 +1189,9 @@
         <f aca="false">H19*G19</f>
         <v>0.52</v>
       </c>
+      <c r="J19" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1122,13 +1201,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>11.32</v>
@@ -1141,7 +1220,7 @@
         <v>22.64</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,13 +1231,13 @@
         <v>6</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>0.1</v>
@@ -1170,6 +1249,9 @@
         <f aca="false">H21*G21</f>
         <v>0.5</v>
       </c>
+      <c r="J21" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -1179,13 +1261,13 @@
         <v>6</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>0.079</v>
@@ -1197,6 +1279,9 @@
         <f aca="false">H22*G22</f>
         <v>0.79</v>
       </c>
+      <c r="J22" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -1206,13 +1291,13 @@
         <v>6</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>0.55</v>
@@ -1224,6 +1309,9 @@
         <f aca="false">H23*G23</f>
         <v>1.65</v>
       </c>
+      <c r="J23" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -1233,13 +1321,13 @@
         <v>6</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>2.61</v>
@@ -1252,7 +1340,7 @@
         <v>5.22</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,13 +1351,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>0.31</v>
@@ -1281,6 +1369,9 @@
         <f aca="false">H25*G25</f>
         <v>0.62</v>
       </c>
+      <c r="J25" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -1290,13 +1381,13 @@
         <v>6</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>0.265</v>
@@ -1309,7 +1400,7 @@
         <v>2.65</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1320,13 +1411,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>0.34</v>
@@ -1339,7 +1430,7 @@
         <v>2.04</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,13 +1441,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>0.33</v>
@@ -1369,7 +1460,7 @@
         <v>1.98</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,13 +1471,13 @@
         <v>6</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>0.0088</v>
@@ -1398,6 +1489,12 @@
         <f aca="false">H29*G29</f>
         <v>0.264</v>
       </c>
+      <c r="J29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -1407,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>0.31</v>
@@ -1425,6 +1522,9 @@
         <f aca="false">H30*G30</f>
         <v>1.24</v>
       </c>
+      <c r="J30" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -1434,13 +1534,13 @@
         <v>6</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>0.249</v>
@@ -1452,6 +1552,9 @@
         <f aca="false">H31*G31</f>
         <v>2.988</v>
       </c>
+      <c r="J31" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -1461,13 +1564,13 @@
         <v>6</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>0.05</v>
@@ -1479,6 +1582,9 @@
         <f aca="false">H32*G32</f>
         <v>0.8</v>
       </c>
+      <c r="J32" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -1488,13 +1594,13 @@
         <v>6</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>0.018</v>
@@ -1507,10 +1613,10 @@
         <v>0.72</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,13 +1627,13 @@
         <v>6</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>0.07</v>
@@ -1539,6 +1645,12 @@
         <f aca="false">H34*G34</f>
         <v>0.35</v>
       </c>
+      <c r="J34" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -1548,13 +1660,13 @@
         <v>6</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>0.07</v>
@@ -1566,6 +1678,12 @@
         <f aca="false">H35*G35</f>
         <v>0.28</v>
       </c>
+      <c r="J35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -1575,13 +1693,13 @@
         <v>6</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>0.07</v>
@@ -1593,6 +1711,12 @@
         <f aca="false">H36*G36</f>
         <v>0.28</v>
       </c>
+      <c r="J36" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -1602,13 +1726,13 @@
         <v>6</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>0.018</v>
@@ -1620,6 +1744,9 @@
         <f aca="false">H37*G37</f>
         <v>0.27</v>
       </c>
+      <c r="J37" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -1629,13 +1756,13 @@
         <v>6</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>0.07</v>
@@ -1647,6 +1774,9 @@
         <f aca="false">H38*G38</f>
         <v>0.14</v>
       </c>
+      <c r="J38" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -1656,13 +1786,13 @@
         <v>6</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G39" s="0" t="n">
         <v>1.01</v>
@@ -1675,7 +1805,7 @@
         <v>2.02</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,13 +1816,13 @@
         <v>6</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>0.55</v>
@@ -1704,6 +1834,9 @@
         <f aca="false">H40*G40</f>
         <v>1.1</v>
       </c>
+      <c r="J40" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -1713,13 +1846,13 @@
         <v>6</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G41" s="0" t="n">
         <v>3.53</v>
@@ -1732,7 +1865,7 @@
         <v>7.06</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1743,13 +1876,13 @@
         <v>6</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="G42" s="0" t="n">
         <v>3.41</v>
@@ -1762,7 +1895,7 @@
         <v>6.82</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,13 +1906,13 @@
         <v>6</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G43" s="0" t="n">
         <v>0.38</v>
@@ -1791,6 +1924,9 @@
         <f aca="false">H43*G43</f>
         <v>0.76</v>
       </c>
+      <c r="J43" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -1800,13 +1936,13 @@
         <v>6</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>0.66</v>
@@ -1819,7 +1955,7 @@
         <v>1.32</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,13 +1966,13 @@
         <v>6</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G45" s="0" t="n">
         <v>2.25</v>
@@ -1848,6 +1984,9 @@
         <f aca="false">H45*G45</f>
         <v>4.5</v>
       </c>
+      <c r="J45" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -1857,13 +1996,13 @@
         <v>6</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>1.41</v>
@@ -1876,7 +2015,7 @@
         <v>2.82</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,13 +2026,13 @@
         <v>6</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="G47" s="0" t="n">
         <v>0.29</v>
@@ -1905,6 +2044,9 @@
         <f aca="false">H47*G47</f>
         <v>0.58</v>
       </c>
+      <c r="J47" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -1914,13 +2056,13 @@
         <v>6</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="G48" s="0" t="n">
         <v>0.44</v>
@@ -1932,6 +2074,12 @@
         <f aca="false">H48*G48</f>
         <v>0.88</v>
       </c>
+      <c r="J48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -1941,13 +2089,13 @@
         <v>6</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="G49" s="0" t="n">
         <v>2.09</v>
@@ -1959,6 +2107,9 @@
         <f aca="false">H49*G49</f>
         <v>4.18</v>
       </c>
+      <c r="J49" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -1968,13 +2119,13 @@
         <v>6</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>0.85</v>
@@ -1986,22 +2137,25 @@
         <f aca="false">H50*G50</f>
         <v>1.7</v>
       </c>
+      <c r="J50" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,16 +2163,16 @@
         <v>2</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,7 +2180,7 @@
         <v>156</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="I53" s="0" t="n">
         <f aca="false">SUM(I2:I50)</f>
@@ -2038,7 +2192,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="G55" s="0" t="n">
         <v>49</v>
@@ -2053,7 +2207,7 @@
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H56" s="0" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="I56" s="0" t="n">
         <f aca="false">I55+I53</f>

</xml_diff>

<commit_message>
update BOM, now finished
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="167">
   <si>
     <t xml:space="preserve">QTY </t>
   </si>
@@ -94,12 +94,12 @@
     <t xml:space="preserve">1u</t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
     <t xml:space="preserve">Got 1</t>
   </si>
   <si>
+    <t xml:space="preserve">now got 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">SML-H12P8TT86CCT-ND</t>
   </si>
   <si>
@@ -166,6 +166,9 @@
     <t xml:space="preserve">camera connector</t>
   </si>
   <si>
+    <t xml:space="preserve">Have now got 2 more</t>
+  </si>
+  <si>
     <t xml:space="preserve">732-2739-1-ND</t>
   </si>
   <si>
@@ -368,6 +371,9 @@
   </si>
   <si>
     <t xml:space="preserve">none arrived</t>
+  </si>
+  <si>
+    <t xml:space="preserve">now have 10</t>
   </si>
   <si>
     <t xml:space="preserve">311-47.0KHRCT-ND</t>
@@ -612,10 +618,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+      <selection pane="topLeft" activeCell="L36" activeCellId="0" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -800,9 +806,12 @@
         <v>0.22</v>
       </c>
       <c r="J6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="L6" s="0" t="s">
         <v>25</v>
       </c>
     </row>
@@ -913,8 +922,10 @@
         <v>38</v>
       </c>
       <c r="I10" s="0" t="n">
-        <f aca="false">H10*G10</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,10 +1015,13 @@
         <v>2.28</v>
       </c>
       <c r="J13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="K13" s="0" t="s">
-        <v>25</v>
+      <c r="L13" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1018,13 +1032,13 @@
         <v>6</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>2.3</v>
@@ -1040,7 +1054,7 @@
         <v>10</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1051,13 +1065,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>0.08</v>
@@ -1081,13 +1095,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>0.1</v>
@@ -1111,13 +1125,13 @@
         <v>6</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>0.14</v>
@@ -1141,13 +1155,13 @@
         <v>6</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>0.2</v>
@@ -1171,13 +1185,13 @@
         <v>6</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>0.26</v>
@@ -1201,13 +1215,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>11.32</v>
@@ -1231,13 +1245,13 @@
         <v>6</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>0.1</v>
@@ -1261,13 +1275,13 @@
         <v>6</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>0.079</v>
@@ -1291,13 +1305,13 @@
         <v>6</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>0.55</v>
@@ -1321,13 +1335,13 @@
         <v>6</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>2.61</v>
@@ -1351,13 +1365,13 @@
         <v>6</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G25" s="0" t="n">
         <v>0.31</v>
@@ -1381,13 +1395,13 @@
         <v>6</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>0.265</v>
@@ -1411,13 +1425,13 @@
         <v>6</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>0.34</v>
@@ -1441,13 +1455,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>0.33</v>
@@ -1471,13 +1485,13 @@
         <v>6</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>0.0088</v>
@@ -1493,7 +1507,7 @@
         <v>10</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,13 +1518,13 @@
         <v>6</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>0.31</v>
@@ -1534,13 +1548,13 @@
         <v>6</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>0.249</v>
@@ -1564,13 +1578,13 @@
         <v>6</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>0.05</v>
@@ -1594,13 +1608,13 @@
         <v>6</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>0.018</v>
@@ -1616,7 +1630,7 @@
         <v>10</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,13 +1641,13 @@
         <v>6</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>0.07</v>
@@ -1649,7 +1663,7 @@
         <v>10</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1660,13 +1674,13 @@
         <v>6</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>0.07</v>
@@ -1682,7 +1696,7 @@
         <v>10</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1693,13 +1707,13 @@
         <v>6</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>0.07</v>
@@ -1712,10 +1726,13 @@
         <v>0.28</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,13 +1743,13 @@
         <v>6</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>0.018</v>
@@ -1756,13 +1773,13 @@
         <v>6</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G38" s="0" t="n">
         <v>0.07</v>
@@ -1786,13 +1803,13 @@
         <v>6</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G39" s="0" t="n">
         <v>1.01</v>
@@ -1816,13 +1833,13 @@
         <v>6</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G40" s="0" t="n">
         <v>0.55</v>
@@ -1846,13 +1863,13 @@
         <v>6</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G41" s="0" t="n">
         <v>3.53</v>
@@ -1876,13 +1893,13 @@
         <v>6</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G42" s="0" t="n">
         <v>3.41</v>
@@ -1906,13 +1923,13 @@
         <v>6</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G43" s="0" t="n">
         <v>0.38</v>
@@ -1936,13 +1953,13 @@
         <v>6</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="G44" s="0" t="n">
         <v>0.66</v>
@@ -1966,13 +1983,13 @@
         <v>6</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G45" s="0" t="n">
         <v>2.25</v>
@@ -1996,13 +2013,13 @@
         <v>6</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G46" s="0" t="n">
         <v>1.41</v>
@@ -2026,13 +2043,13 @@
         <v>6</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G47" s="0" t="n">
         <v>0.29</v>
@@ -2056,13 +2073,13 @@
         <v>6</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G48" s="0" t="n">
         <v>0.44</v>
@@ -2078,7 +2095,7 @@
         <v>10</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,13 +2106,13 @@
         <v>6</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G49" s="0" t="n">
         <v>2.09</v>
@@ -2119,13 +2136,13 @@
         <v>6</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G50" s="0" t="n">
         <v>0.85</v>
@@ -2146,16 +2163,16 @@
         <v>4</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2163,16 +2180,16 @@
         <v>2</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,11 +2197,11 @@
         <v>156</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="I53" s="0" t="n">
         <f aca="false">SUM(I2:I50)</f>
-        <v>125.2824</v>
+        <v>127.2824</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,7 +2209,7 @@
         <v>2</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G55" s="0" t="n">
         <v>49</v>
@@ -2207,11 +2224,11 @@
     </row>
     <row r="56" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H56" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I56" s="0" t="n">
         <f aca="false">I55+I53</f>
-        <v>223.2824</v>
+        <v>225.2824</v>
       </c>
     </row>
   </sheetData>

</xml_diff>